<commit_message>
Clean python project structure.
</commit_message>
<xml_diff>
--- a/data/input/data_pitch.xlsx
+++ b/data/input/data_pitch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cosmicthermo/Desktop/Afairi-Work/Github/Simulation_UW/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FC29BF-DB42-5542-965E-4D12345A6C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C488020E-7100-F94E-9CDB-1DD9F58189D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="500" windowWidth="25160" windowHeight="19700" activeTab="5" xr2:uid="{EAAEE87E-042B-8C4D-B52E-B80F51B8DCF5}"/>
+    <workbookView xWindow="9020" yWindow="500" windowWidth="25160" windowHeight="17500" activeTab="4" xr2:uid="{EAAEE87E-042B-8C4D-B52E-B80F51B8DCF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1280,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5266D9FA-80CC-CB42-9602-93779702D86C}">
   <dimension ref="A1:T66"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView topLeftCell="C1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2788,7 +2788,7 @@
   <dimension ref="A1:EK65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2887,7 +2887,7 @@
         <v>187</v>
       </c>
       <c r="H4" s="44">
-        <v>611870.66666666674</v>
+        <v>16972.666666666672</v>
       </c>
     </row>
     <row r="5" spans="1:141" x14ac:dyDescent="0.2">
@@ -2901,8 +2901,8 @@
       <c r="G5" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="17">
-        <v>300.00000000000006</v>
+      <c r="H5" s="26">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:141" x14ac:dyDescent="0.2">
@@ -4155,7 +4155,7 @@
   <dimension ref="A1:EK65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4254,7 +4254,7 @@
         <v>187</v>
       </c>
       <c r="H4" s="44">
-        <v>865382.66666666674</v>
+        <v>21126</v>
       </c>
     </row>
     <row r="5" spans="1:141" x14ac:dyDescent="0.2">
@@ -4268,8 +4268,8 @@
       <c r="G5" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="17">
-        <v>303.33333333333337</v>
+      <c r="H5" s="26">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:141" x14ac:dyDescent="0.2">
@@ -9346,7 +9346,7 @@
   <dimension ref="A1:EK65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9445,7 +9445,7 @@
         <v>187</v>
       </c>
       <c r="H4" s="44">
-        <v>2100</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:141" x14ac:dyDescent="0.2">
@@ -9460,7 +9460,7 @@
         <v>188</v>
       </c>
       <c r="H5" s="17">
-        <v>360</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:141" x14ac:dyDescent="0.2">
@@ -10713,8 +10713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009401E7-806E-9048-AF25-ABF9F1BC7F69}">
   <dimension ref="A1:EK65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10813,7 +10813,7 @@
         <v>187</v>
       </c>
       <c r="H4" s="44">
-        <v>15790.666666666666</v>
+        <v>1140.8888888888916</v>
       </c>
     </row>
     <row r="5" spans="1:141" x14ac:dyDescent="0.2">
@@ -10827,8 +10827,8 @@
       <c r="G5" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="17">
-        <v>350</v>
+      <c r="H5" s="26">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:141" x14ac:dyDescent="0.2">
@@ -12080,8 +12080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8539A6F3-8246-344D-A1FE-14B9DE6FF450}">
   <dimension ref="A1:EK65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12180,7 +12180,7 @@
         <v>187</v>
       </c>
       <c r="H4" s="44">
-        <v>52014.666666666701</v>
+        <v>3018.6666666666638</v>
       </c>
     </row>
     <row r="5" spans="1:141" x14ac:dyDescent="0.2">
@@ -12194,8 +12194,8 @@
       <c r="G5" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="17">
-        <v>306.25</v>
+      <c r="H5" s="26">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:141" x14ac:dyDescent="0.2">
@@ -13448,7 +13448,7 @@
   <dimension ref="A1:EK65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13547,7 +13547,7 @@
         <v>187</v>
       </c>
       <c r="H4" s="44">
-        <v>125214.66666666666</v>
+        <v>6100</v>
       </c>
     </row>
     <row r="5" spans="1:141" x14ac:dyDescent="0.2">
@@ -13561,8 +13561,8 @@
       <c r="G5" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="17">
-        <v>262.5</v>
+      <c r="H5" s="26">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:141" x14ac:dyDescent="0.2">
@@ -14815,7 +14815,7 @@
   <dimension ref="A1:EK65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14914,7 +14914,7 @@
         <v>187</v>
       </c>
       <c r="H4" s="44">
-        <v>251678.66666666666</v>
+        <v>10538.666666666666</v>
       </c>
     </row>
     <row r="5" spans="1:141" x14ac:dyDescent="0.2">
@@ -14928,8 +14928,8 @@
       <c r="G5" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="17">
-        <v>291.66666666666663</v>
+      <c r="H5" s="26">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:141" x14ac:dyDescent="0.2">
@@ -16182,7 +16182,7 @@
   <dimension ref="A1:EK65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16281,7 +16281,7 @@
         <v>187</v>
       </c>
       <c r="H4" s="44">
-        <v>408198.66666666669</v>
+        <v>13043.333333333336</v>
       </c>
     </row>
     <row r="5" spans="1:141" x14ac:dyDescent="0.2">
@@ -16295,8 +16295,8 @@
       <c r="G5" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="17">
-        <v>296.15384615384619</v>
+      <c r="H5" s="26">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:141" x14ac:dyDescent="0.2">

</xml_diff>